<commit_message>
debug basic enhancement, add munsell test and correct color name table
</commit_message>
<xml_diff>
--- a/name_table.xlsx
+++ b/name_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65b8bda2390db6a6/CIE_CURVE/color_names/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_AD4DA82427541F7ACA7EB857104D3AC06BE8DE17" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1088F949-CA6A-4196-A4CC-22BFD04F9A1F}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_AD4DA82427541F7ACA7EB857104D3AC06BE8DE17" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF3ADD0C-D01E-485F-BB83-2B5F9465D0AC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'表 1'!$A$1:$D$171</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'表 1'!$A$1:$D$145</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="435">
   <si>
     <t>HEX</t>
   </si>
@@ -1331,10 +1331,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Cyan</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>White</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1347,186 +1343,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>70,70,70</t>
-  </si>
-  <si>
-    <t>80,80,80</t>
-  </si>
-  <si>
-    <t>90,90,90</t>
-  </si>
-  <si>
-    <t>255,160,64</t>
+    <t>Blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Green</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Orange</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>255,160,96</t>
-  </si>
-  <si>
-    <t>130,130,130</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>150,150,150</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>255,160,160</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>255,192,160</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>255,96,0</t>
-  </si>
-  <si>
-    <t>255,96,128</t>
-  </si>
-  <si>
-    <t>224,255,64</t>
-  </si>
-  <si>
-    <t>224,160,160</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>224,64,32</t>
-  </si>
-  <si>
-    <t>Red</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>224,0,192</t>
-  </si>
-  <si>
-    <t>192,192,32</t>
-  </si>
-  <si>
-    <t>192,255,192</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Green</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>192,192,0</t>
-  </si>
-  <si>
-    <t>160,192,96</t>
-  </si>
-  <si>
-    <t>160,224,192</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>128,64,96</t>
-  </si>
-  <si>
-    <t>128,96,160</t>
-  </si>
-  <si>
-    <t>96,64,64</t>
-  </si>
-  <si>
-    <t>64,64,160</t>
-  </si>
-  <si>
-    <t>Blue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>64,0,0</t>
-  </si>
-  <si>
-    <t>AP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AP0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AP24</t>
-  </si>
-  <si>
-    <t>AP1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AP2</t>
-  </si>
-  <si>
-    <t>AP3</t>
-  </si>
-  <si>
-    <t>AP4</t>
-  </si>
-  <si>
-    <t>AP5</t>
-  </si>
-  <si>
-    <t>AP6</t>
-  </si>
-  <si>
-    <t>AP7</t>
-  </si>
-  <si>
-    <t>AP8</t>
-  </si>
-  <si>
-    <t>AP9</t>
-  </si>
-  <si>
-    <t>AP10</t>
-  </si>
-  <si>
-    <t>AP11</t>
-  </si>
-  <si>
-    <t>AP12</t>
-  </si>
-  <si>
-    <t>AP13</t>
-  </si>
-  <si>
-    <t>AP14</t>
-  </si>
-  <si>
-    <t>AP15</t>
-  </si>
-  <si>
-    <t>AP16</t>
-  </si>
-  <si>
-    <t>AP17</t>
-  </si>
-  <si>
-    <t>AP18</t>
-  </si>
-  <si>
-    <t>AP19</t>
-  </si>
-  <si>
-    <t>AP20</t>
-  </si>
-  <si>
-    <t>AP21</t>
-  </si>
-  <si>
-    <t>AP22</t>
-  </si>
-  <si>
-    <t>AP23</t>
-  </si>
-  <si>
-    <t>AP25</t>
   </si>
 </sst>
 </file>
@@ -1569,11 +1395,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1618,8 +1442,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E9C9674-90CE-4D8F-B127-5F27C9B931F5}" name="表_1" displayName="表_1" ref="A1:D171" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D171" xr:uid="{5E9C9674-90CE-4D8F-B127-5F27C9B931F5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E9C9674-90CE-4D8F-B127-5F27C9B931F5}" name="表_1" displayName="表_1" ref="A1:D145" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D145" xr:uid="{5E9C9674-90CE-4D8F-B127-5F27C9B931F5}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A71A95BF-58BF-4D55-8E8C-2208518EE4D6}" uniqueName="1" name="Colorname" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{E612895B-8433-425C-99DA-B7549524A36F}" uniqueName="2" name="HEX" queryTableFieldId="2" dataDxfId="2"/>
@@ -1895,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41BA6CDF-51E5-4163-9A88-E70DDB856298}">
   <dimension ref="A1:D171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146:A171"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1918,7 +1742,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1928,11 +1752,11 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>285</v>
       </c>
       <c r="D2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1942,7 +1766,7 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>286</v>
       </c>
       <c r="D3" t="s">
@@ -1956,11 +1780,11 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>287</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1970,11 +1794,11 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>288</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>433</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1984,11 +1808,11 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>289</v>
       </c>
       <c r="D6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1998,11 +1822,11 @@
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>290</v>
       </c>
       <c r="D7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2012,7 +1836,7 @@
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>291</v>
       </c>
       <c r="D8" t="s">
@@ -2026,7 +1850,7 @@
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>292</v>
       </c>
       <c r="D9" t="s">
@@ -2040,7 +1864,7 @@
       <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>293</v>
       </c>
       <c r="D10" t="s">
@@ -2054,7 +1878,7 @@
       <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>294</v>
       </c>
       <c r="D11" t="s">
@@ -2068,7 +1892,7 @@
       <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>295</v>
       </c>
       <c r="D12" t="s">
@@ -2082,7 +1906,7 @@
       <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>296</v>
       </c>
       <c r="D13" t="s">
@@ -2096,7 +1920,7 @@
       <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>297</v>
       </c>
       <c r="D14" t="s">
@@ -2110,11 +1934,11 @@
       <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>298</v>
       </c>
       <c r="D15" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2124,7 +1948,7 @@
       <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>299</v>
       </c>
       <c r="D16" t="s">
@@ -2138,11 +1962,11 @@
       <c r="B17" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>300</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>434</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2152,7 +1976,7 @@
       <c r="B18" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>301</v>
       </c>
       <c r="D18" t="s">
@@ -2166,7 +1990,7 @@
       <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>302</v>
       </c>
       <c r="D19" t="s">
@@ -2180,7 +2004,7 @@
       <c r="B20" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>303</v>
       </c>
       <c r="D20" t="s">
@@ -2194,7 +2018,7 @@
       <c r="B21" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>304</v>
       </c>
       <c r="D21" t="s">
@@ -2208,11 +2032,11 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>287</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>432</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2222,7 +2046,7 @@
       <c r="B23" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>305</v>
       </c>
       <c r="D23" t="s">
@@ -2236,11 +2060,11 @@
       <c r="B24" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>306</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>433</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2250,7 +2074,7 @@
       <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>307</v>
       </c>
       <c r="D25" t="s">
@@ -2264,7 +2088,7 @@
       <c r="B26" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>308</v>
       </c>
       <c r="D26" t="s">
@@ -2278,7 +2102,7 @@
       <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>309</v>
       </c>
       <c r="D27" t="s">
@@ -2292,7 +2116,7 @@
       <c r="B28" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>310</v>
       </c>
       <c r="D28" t="s">
@@ -2306,7 +2130,7 @@
       <c r="B29" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>311</v>
       </c>
       <c r="D29" t="s">
@@ -2320,7 +2144,7 @@
       <c r="B30" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>312</v>
       </c>
       <c r="D30" t="s">
@@ -2334,7 +2158,7 @@
       <c r="B31" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>313</v>
       </c>
       <c r="D31" t="s">
@@ -2348,7 +2172,7 @@
       <c r="B32" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>314</v>
       </c>
       <c r="D32" t="s">
@@ -2362,7 +2186,7 @@
       <c r="B33" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>315</v>
       </c>
       <c r="D33" t="s">
@@ -2376,7 +2200,7 @@
       <c r="B34" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>316</v>
       </c>
       <c r="D34" t="s">
@@ -2390,7 +2214,7 @@
       <c r="B35" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>317</v>
       </c>
       <c r="D35" t="s">
@@ -2404,7 +2228,7 @@
       <c r="B36" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>318</v>
       </c>
       <c r="D36" t="s">
@@ -2418,11 +2242,11 @@
       <c r="B37" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>319</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>432</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2432,11 +2256,11 @@
       <c r="B38" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>319</v>
       </c>
       <c r="D38" t="s">
-        <v>57</v>
+        <v>432</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2446,11 +2270,11 @@
       <c r="B39" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>320</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>432</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2460,7 +2284,7 @@
       <c r="B40" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>321</v>
       </c>
       <c r="D40" t="s">
@@ -2474,7 +2298,7 @@
       <c r="B41" t="s">
         <v>86</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>322</v>
       </c>
       <c r="D41" t="s">
@@ -2488,7 +2312,7 @@
       <c r="B42" t="s">
         <v>89</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>323</v>
       </c>
       <c r="D42" t="s">
@@ -2502,7 +2326,7 @@
       <c r="B43" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>324</v>
       </c>
       <c r="D43" t="s">
@@ -2516,7 +2340,7 @@
       <c r="B44" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>325</v>
       </c>
       <c r="D44" t="s">
@@ -2530,7 +2354,7 @@
       <c r="B45" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>326</v>
       </c>
       <c r="D45" t="s">
@@ -2544,7 +2368,7 @@
       <c r="B46" t="s">
         <v>97</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>327</v>
       </c>
       <c r="D46" t="s">
@@ -2558,7 +2382,7 @@
       <c r="B47" t="s">
         <v>99</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>328</v>
       </c>
       <c r="D47" t="s">
@@ -2572,7 +2396,7 @@
       <c r="B48" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>329</v>
       </c>
       <c r="D48" t="s">
@@ -2586,11 +2410,11 @@
       <c r="B49" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>330</v>
       </c>
       <c r="D49" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2600,7 +2424,7 @@
       <c r="B50" t="s">
         <v>105</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>331</v>
       </c>
       <c r="D50" t="s">
@@ -2614,7 +2438,7 @@
       <c r="B51" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>332</v>
       </c>
       <c r="D51" t="s">
@@ -2628,11 +2452,11 @@
       <c r="B52" t="s">
         <v>109</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>333</v>
       </c>
       <c r="D52" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2642,7 +2466,7 @@
       <c r="B53" t="s">
         <v>110</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>334</v>
       </c>
       <c r="D53" t="s">
@@ -2656,7 +2480,7 @@
       <c r="B54" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>335</v>
       </c>
       <c r="D54" t="s">
@@ -2670,7 +2494,7 @@
       <c r="B55" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="1" t="s">
         <v>336</v>
       </c>
       <c r="D55" t="s">
@@ -2684,7 +2508,7 @@
       <c r="B56" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>337</v>
       </c>
       <c r="D56" t="s">
@@ -2698,7 +2522,7 @@
       <c r="B57" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="1" t="s">
         <v>338</v>
       </c>
       <c r="D57" t="s">
@@ -2712,7 +2536,7 @@
       <c r="B58" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="1" t="s">
         <v>339</v>
       </c>
       <c r="D58" t="s">
@@ -2726,7 +2550,7 @@
       <c r="B59" t="s">
         <v>121</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="1" t="s">
         <v>340</v>
       </c>
       <c r="D59" t="s">
@@ -2740,7 +2564,7 @@
       <c r="B60" t="s">
         <v>123</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>341</v>
       </c>
       <c r="D60" t="s">
@@ -2754,7 +2578,7 @@
       <c r="B61" t="s">
         <v>125</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="1" t="s">
         <v>342</v>
       </c>
       <c r="D61" t="s">
@@ -2768,7 +2592,7 @@
       <c r="B62" t="s">
         <v>127</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="1" t="s">
         <v>343</v>
       </c>
       <c r="D62" t="s">
@@ -2782,11 +2606,11 @@
       <c r="B63" t="s">
         <v>129</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="1" t="s">
         <v>344</v>
       </c>
       <c r="D63" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2796,7 +2620,7 @@
       <c r="B64" t="s">
         <v>131</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="1" t="s">
         <v>345</v>
       </c>
       <c r="D64" t="s">
@@ -2810,7 +2634,7 @@
       <c r="B65" t="s">
         <v>133</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="1" t="s">
         <v>346</v>
       </c>
       <c r="D65" t="s">
@@ -2824,7 +2648,7 @@
       <c r="B66" t="s">
         <v>135</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="1" t="s">
         <v>347</v>
       </c>
       <c r="D66" t="s">
@@ -2838,7 +2662,7 @@
       <c r="B67" t="s">
         <v>137</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="1" t="s">
         <v>348</v>
       </c>
       <c r="D67" t="s">
@@ -2852,11 +2676,11 @@
       <c r="B68" t="s">
         <v>139</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>349</v>
       </c>
       <c r="D68" t="s">
-        <v>10</v>
+        <v>432</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2866,7 +2690,7 @@
       <c r="B69" t="s">
         <v>141</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="1" t="s">
         <v>350</v>
       </c>
       <c r="D69" t="s">
@@ -2880,7 +2704,7 @@
       <c r="B70" t="s">
         <v>143</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="1" t="s">
         <v>351</v>
       </c>
       <c r="D70" t="s">
@@ -2894,7 +2718,7 @@
       <c r="B71" t="s">
         <v>145</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="1" t="s">
         <v>352</v>
       </c>
       <c r="D71" t="s">
@@ -2908,7 +2732,7 @@
       <c r="B72" t="s">
         <v>147</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="1" t="s">
         <v>353</v>
       </c>
       <c r="D72" t="s">
@@ -2922,7 +2746,7 @@
       <c r="B73" t="s">
         <v>149</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="1" t="s">
         <v>354</v>
       </c>
       <c r="D73" t="s">
@@ -2936,11 +2760,11 @@
       <c r="B74" t="s">
         <v>151</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="1" t="s">
         <v>355</v>
       </c>
       <c r="D74" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2950,7 +2774,7 @@
       <c r="B75" t="s">
         <v>153</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="1" t="s">
         <v>356</v>
       </c>
       <c r="D75" t="s">
@@ -2964,7 +2788,7 @@
       <c r="B76" t="s">
         <v>155</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="1" t="s">
         <v>357</v>
       </c>
       <c r="D76" t="s">
@@ -2978,7 +2802,7 @@
       <c r="B77" t="s">
         <v>155</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="1" t="s">
         <v>357</v>
       </c>
       <c r="D77" t="s">
@@ -2992,7 +2816,7 @@
       <c r="B78" t="s">
         <v>158</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="1" t="s">
         <v>358</v>
       </c>
       <c r="D78" t="s">
@@ -3006,7 +2830,7 @@
       <c r="B79" t="s">
         <v>160</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="1" t="s">
         <v>359</v>
       </c>
       <c r="D79" t="s">
@@ -3020,7 +2844,7 @@
       <c r="B80" t="s">
         <v>162</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="1" t="s">
         <v>360</v>
       </c>
       <c r="D80" t="s">
@@ -3034,7 +2858,7 @@
       <c r="B81" t="s">
         <v>164</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="1" t="s">
         <v>361</v>
       </c>
       <c r="D81" t="s">
@@ -3048,11 +2872,11 @@
       <c r="B82" t="s">
         <v>166</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="1" t="s">
         <v>362</v>
       </c>
       <c r="D82" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -3062,7 +2886,7 @@
       <c r="B83" t="s">
         <v>101</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="1" t="s">
         <v>329</v>
       </c>
       <c r="D83" t="s">
@@ -3076,7 +2900,7 @@
       <c r="B84" t="s">
         <v>169</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="1" t="s">
         <v>363</v>
       </c>
       <c r="D84" t="s">
@@ -3090,11 +2914,11 @@
       <c r="B85" t="s">
         <v>171</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="1" t="s">
         <v>364</v>
       </c>
       <c r="D85" t="s">
-        <v>10</v>
+        <v>433</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -3104,7 +2928,7 @@
       <c r="B86" t="s">
         <v>173</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="1" t="s">
         <v>365</v>
       </c>
       <c r="D86" t="s">
@@ -3118,7 +2942,7 @@
       <c r="B87" t="s">
         <v>175</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="1" t="s">
         <v>366</v>
       </c>
       <c r="D87" t="s">
@@ -3132,7 +2956,7 @@
       <c r="B88" t="s">
         <v>177</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="1" t="s">
         <v>367</v>
       </c>
       <c r="D88" t="s">
@@ -3146,7 +2970,7 @@
       <c r="B89" t="s">
         <v>179</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="1" t="s">
         <v>368</v>
       </c>
       <c r="D89" t="s">
@@ -3160,7 +2984,7 @@
       <c r="B90" t="s">
         <v>181</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="1" t="s">
         <v>369</v>
       </c>
       <c r="D90" t="s">
@@ -3174,7 +2998,7 @@
       <c r="B91" t="s">
         <v>183</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="1" t="s">
         <v>370</v>
       </c>
       <c r="D91" t="s">
@@ -3188,11 +3012,11 @@
       <c r="B92" t="s">
         <v>185</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="1" t="s">
         <v>371</v>
       </c>
       <c r="D92" t="s">
-        <v>10</v>
+        <v>432</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -3202,7 +3026,7 @@
       <c r="B93" t="s">
         <v>187</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="1" t="s">
         <v>372</v>
       </c>
       <c r="D93" t="s">
@@ -3216,7 +3040,7 @@
       <c r="B94" t="s">
         <v>189</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="1" t="s">
         <v>373</v>
       </c>
       <c r="D94" t="s">
@@ -3230,7 +3054,7 @@
       <c r="B95" t="s">
         <v>191</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C95" s="1" t="s">
         <v>374</v>
       </c>
       <c r="D95" t="s">
@@ -3244,7 +3068,7 @@
       <c r="B96" t="s">
         <v>193</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C96" s="1" t="s">
         <v>375</v>
       </c>
       <c r="D96" t="s">
@@ -3258,7 +3082,7 @@
       <c r="B97" t="s">
         <v>195</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="1" t="s">
         <v>376</v>
       </c>
       <c r="D97" t="s">
@@ -3272,7 +3096,7 @@
       <c r="B98" t="s">
         <v>197</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C98" s="1" t="s">
         <v>377</v>
       </c>
       <c r="D98" t="s">
@@ -3286,7 +3110,7 @@
       <c r="B99" t="s">
         <v>199</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="1" t="s">
         <v>378</v>
       </c>
       <c r="D99" t="s">
@@ -3300,11 +3124,11 @@
       <c r="B100" t="s">
         <v>201</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C100" s="1" t="s">
         <v>379</v>
       </c>
       <c r="D100" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3314,7 +3138,7 @@
       <c r="B101" t="s">
         <v>203</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C101" s="1" t="s">
         <v>380</v>
       </c>
       <c r="D101" t="s">
@@ -3328,7 +3152,7 @@
       <c r="B102" t="s">
         <v>205</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="1" t="s">
         <v>381</v>
       </c>
       <c r="D102" t="s">
@@ -3342,7 +3166,7 @@
       <c r="B103" t="s">
         <v>206</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C103" s="1" t="s">
         <v>382</v>
       </c>
       <c r="D103" t="s">
@@ -3356,7 +3180,7 @@
       <c r="B104" t="s">
         <v>208</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C104" s="1" t="s">
         <v>383</v>
       </c>
       <c r="D104" t="s">
@@ -3370,7 +3194,7 @@
       <c r="B105" t="s">
         <v>210</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="C105" s="1" t="s">
         <v>384</v>
       </c>
       <c r="D105" t="s">
@@ -3384,7 +3208,7 @@
       <c r="B106" t="s">
         <v>212</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="1" t="s">
         <v>385</v>
       </c>
       <c r="D106" t="s">
@@ -3398,7 +3222,7 @@
       <c r="B107" t="s">
         <v>214</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C107" s="1" t="s">
         <v>386</v>
       </c>
       <c r="D107" t="s">
@@ -3412,11 +3236,11 @@
       <c r="B108" t="s">
         <v>216</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C108" s="1" t="s">
         <v>387</v>
       </c>
       <c r="D108" t="s">
-        <v>10</v>
+        <v>432</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3426,7 +3250,7 @@
       <c r="B109" t="s">
         <v>218</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C109" s="1" t="s">
         <v>388</v>
       </c>
       <c r="D109" t="s">
@@ -3440,7 +3264,7 @@
       <c r="B110" t="s">
         <v>220</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="C110" s="1" t="s">
         <v>389</v>
       </c>
       <c r="D110" t="s">
@@ -3454,7 +3278,7 @@
       <c r="B111" t="s">
         <v>222</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C111" s="1" t="s">
         <v>390</v>
       </c>
       <c r="D111" t="s">
@@ -3468,7 +3292,7 @@
       <c r="B112" t="s">
         <v>224</v>
       </c>
-      <c r="C112" s="2" t="s">
+      <c r="C112" s="1" t="s">
         <v>391</v>
       </c>
       <c r="D112" t="s">
@@ -3482,7 +3306,7 @@
       <c r="B113" t="s">
         <v>225</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="1" t="s">
         <v>392</v>
       </c>
       <c r="D113" t="s">
@@ -3496,7 +3320,7 @@
       <c r="B114" t="s">
         <v>227</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C114" s="1" t="s">
         <v>393</v>
       </c>
       <c r="D114" t="s">
@@ -3510,7 +3334,7 @@
       <c r="B115" t="s">
         <v>229</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="1" t="s">
         <v>394</v>
       </c>
       <c r="D115" t="s">
@@ -3524,7 +3348,7 @@
       <c r="B116" t="s">
         <v>230</v>
       </c>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="1" t="s">
         <v>395</v>
       </c>
       <c r="D116" t="s">
@@ -3538,7 +3362,7 @@
       <c r="B117" t="s">
         <v>232</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="1" t="s">
         <v>396</v>
       </c>
       <c r="D117" t="s">
@@ -3552,7 +3376,7 @@
       <c r="B118" t="s">
         <v>233</v>
       </c>
-      <c r="C118" s="2" t="s">
+      <c r="C118" s="1" t="s">
         <v>397</v>
       </c>
       <c r="D118" t="s">
@@ -3566,7 +3390,7 @@
       <c r="B119" t="s">
         <v>235</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="C119" s="1" t="s">
         <v>398</v>
       </c>
       <c r="D119" t="s">
@@ -3580,7 +3404,7 @@
       <c r="B120" t="s">
         <v>237</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C120" s="1" t="s">
         <v>399</v>
       </c>
       <c r="D120" t="s">
@@ -3594,7 +3418,7 @@
       <c r="B121" t="s">
         <v>239</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="C121" s="1" t="s">
         <v>400</v>
       </c>
       <c r="D121" t="s">
@@ -3608,11 +3432,11 @@
       <c r="B122" t="s">
         <v>241</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="1" t="s">
         <v>401</v>
       </c>
       <c r="D122" t="s">
-        <v>40</v>
+        <v>425</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -3622,7 +3446,7 @@
       <c r="B123" t="s">
         <v>243</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="C123" s="1" t="s">
         <v>402</v>
       </c>
       <c r="D123" t="s">
@@ -3636,7 +3460,7 @@
       <c r="B124" t="s">
         <v>245</v>
       </c>
-      <c r="C124" s="2" t="s">
+      <c r="C124" s="1" t="s">
         <v>403</v>
       </c>
       <c r="D124" t="s">
@@ -3650,11 +3474,11 @@
       <c r="B125" t="s">
         <v>247</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="C125" s="1" t="s">
         <v>404</v>
       </c>
       <c r="D125" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3664,7 +3488,7 @@
       <c r="B126" t="s">
         <v>249</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="C126" s="1" t="s">
         <v>405</v>
       </c>
       <c r="D126" t="s">
@@ -3678,7 +3502,7 @@
       <c r="B127" t="s">
         <v>251</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="C127" s="1" t="s">
         <v>406</v>
       </c>
       <c r="D127" t="s">
@@ -3692,7 +3516,7 @@
       <c r="B128" t="s">
         <v>253</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C128" s="1" t="s">
         <v>407</v>
       </c>
       <c r="D128" t="s">
@@ -3706,7 +3530,7 @@
       <c r="B129" t="s">
         <v>255</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C129" s="1" t="s">
         <v>408</v>
       </c>
       <c r="D129" t="s">
@@ -3720,7 +3544,7 @@
       <c r="B130" t="s">
         <v>257</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="C130" s="1" t="s">
         <v>409</v>
       </c>
       <c r="D130" t="s">
@@ -3734,7 +3558,7 @@
       <c r="B131" t="s">
         <v>257</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="C131" s="1" t="s">
         <v>409</v>
       </c>
       <c r="D131" t="s">
@@ -3748,7 +3572,7 @@
       <c r="B132" t="s">
         <v>260</v>
       </c>
-      <c r="C132" s="2" t="s">
+      <c r="C132" s="1" t="s">
         <v>410</v>
       </c>
       <c r="D132" t="s">
@@ -3762,7 +3586,7 @@
       <c r="B133" t="s">
         <v>262</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C133" s="1" t="s">
         <v>411</v>
       </c>
       <c r="D133" t="s">
@@ -3776,7 +3600,7 @@
       <c r="B134" t="s">
         <v>264</v>
       </c>
-      <c r="C134" s="2" t="s">
+      <c r="C134" s="1" t="s">
         <v>412</v>
       </c>
       <c r="D134" t="s">
@@ -3790,7 +3614,7 @@
       <c r="B135" t="s">
         <v>266</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C135" s="1" t="s">
         <v>413</v>
       </c>
       <c r="D135" t="s">
@@ -3804,11 +3628,11 @@
       <c r="B136" t="s">
         <v>268</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C136" s="1" t="s">
         <v>414</v>
       </c>
       <c r="D136" t="s">
-        <v>10</v>
+        <v>433</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -3818,7 +3642,7 @@
       <c r="B137" t="s">
         <v>270</v>
       </c>
-      <c r="C137" s="2" t="s">
+      <c r="C137" s="1" t="s">
         <v>415</v>
       </c>
       <c r="D137" t="s">
@@ -3832,7 +3656,7 @@
       <c r="B138" t="s">
         <v>272</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C138" s="1" t="s">
         <v>416</v>
       </c>
       <c r="D138" t="s">
@@ -3846,11 +3670,11 @@
       <c r="B139" t="s">
         <v>274</v>
       </c>
-      <c r="C139" s="2" t="s">
+      <c r="C139" s="1" t="s">
         <v>417</v>
       </c>
       <c r="D139" t="s">
-        <v>10</v>
+        <v>432</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3860,7 +3684,7 @@
       <c r="B140" t="s">
         <v>276</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="C140" s="1" t="s">
         <v>418</v>
       </c>
       <c r="D140" t="s">
@@ -3874,7 +3698,7 @@
       <c r="B141" t="s">
         <v>278</v>
       </c>
-      <c r="C141" s="2" t="s">
+      <c r="C141" s="1" t="s">
         <v>419</v>
       </c>
       <c r="D141" t="s">
@@ -3888,7 +3712,7 @@
       <c r="B142" t="s">
         <v>279</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C142" s="1" t="s">
         <v>420</v>
       </c>
       <c r="D142" t="s">
@@ -3902,7 +3726,7 @@
       <c r="B143" t="s">
         <v>281</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="C143" s="1" t="s">
         <v>421</v>
       </c>
       <c r="D143" t="s">
@@ -3916,7 +3740,7 @@
       <c r="B144" t="s">
         <v>282</v>
       </c>
-      <c r="C144" s="2" t="s">
+      <c r="C144" s="1" t="s">
         <v>422</v>
       </c>
       <c r="D144" t="s">
@@ -3930,7 +3754,7 @@
       <c r="B145" t="s">
         <v>284</v>
       </c>
-      <c r="C145" s="2" t="s">
+      <c r="C145" s="1" t="s">
         <v>423</v>
       </c>
       <c r="D145" t="s">
@@ -3938,368 +3762,82 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>431</v>
-      </c>
+      <c r="C146" s="1"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>431</v>
-      </c>
+      <c r="C147" s="1"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="D148" s="1" t="s">
-        <v>431</v>
-      </c>
+      <c r="C148" s="1"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>431</v>
-      </c>
+      <c r="C149" s="1"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C150" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="D150" s="1" t="s">
-        <v>431</v>
-      </c>
+      <c r="C150" s="1"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>437</v>
-      </c>
+      <c r="C151" s="1"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>437</v>
-      </c>
+      <c r="C152" s="1"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C153" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>425</v>
-      </c>
+      <c r="C153" s="1"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>437</v>
-      </c>
+      <c r="C154" s="1"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>437</v>
-      </c>
+      <c r="C155" s="1"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>425</v>
-      </c>
+      <c r="C156" s="1"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>427</v>
-      </c>
+      <c r="C157" s="1"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="D158" s="1" t="s">
-        <v>425</v>
-      </c>
+      <c r="C158" s="1"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C159" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>427</v>
-      </c>
+      <c r="C159" s="1"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C164" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="D168" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>426</v>
-      </c>
+      <c r="C160" s="1"/>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C161" s="1"/>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C162" s="1"/>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C163" s="1"/>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C164" s="1"/>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C165" s="1"/>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C166" s="1"/>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C167" s="1"/>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C168" s="1"/>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C169" s="1"/>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C170" s="1"/>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C171" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update color naming rules
</commit_message>
<xml_diff>
--- a/name_table.xlsx
+++ b/name_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65b8bda2390db6a6/CIE_CURVE/color_names/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_AD4DA82427541F7ACA7EB857104D3AC06BE8DE17" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF3ADD0C-D01E-485F-BB83-2B5F9465D0AC}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="11_AD4DA82427541F7ACA7EB857104D3AC06BE8DE17" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57B08D0A-6B43-4FF9-A166-BC2D4DF3ED4C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'表 1'!$A$1:$D$145</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'表 1'!$A$1:$D$171</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="482">
   <si>
     <t>HEX</t>
   </si>
@@ -204,15 +204,6 @@
     <t>Yellow</t>
   </si>
   <si>
-    <t>DarkGray</t>
-  </si>
-  <si>
-    <t>A9A9A9</t>
-  </si>
-  <si>
-    <t>Gray</t>
-  </si>
-  <si>
     <t>DarkGreen</t>
   </si>
   <si>
@@ -279,9 +270,6 @@
     <t>2F4F4F</t>
   </si>
   <si>
-    <t>DarkSlateGrey</t>
-  </si>
-  <si>
     <t>DarkTurquoise</t>
   </si>
   <si>
@@ -309,12 +297,6 @@
     <t>00BFFF</t>
   </si>
   <si>
-    <t>DimGray</t>
-  </si>
-  <si>
-    <t>696969</t>
-  </si>
-  <si>
     <t>DodgerBlue</t>
   </si>
   <si>
@@ -345,12 +327,6 @@
     <t>FF00FF</t>
   </si>
   <si>
-    <t>Gainsboro</t>
-  </si>
-  <si>
-    <t>DCDCDC</t>
-  </si>
-  <si>
     <t>GhostWhite</t>
   </si>
   <si>
@@ -369,9 +345,6 @@
     <t>DAA520</t>
   </si>
   <si>
-    <t>808080</t>
-  </si>
-  <si>
     <t>008000</t>
   </si>
   <si>
@@ -465,12 +438,6 @@
     <t>FAFAD2</t>
   </si>
   <si>
-    <t>LightGray</t>
-  </si>
-  <si>
-    <t>D3D3D3</t>
-  </si>
-  <si>
     <t>LightGreen</t>
   </si>
   <si>
@@ -501,15 +468,6 @@
     <t>87CEFA</t>
   </si>
   <si>
-    <t>LightSlateGray</t>
-  </si>
-  <si>
-    <t>778899</t>
-  </si>
-  <si>
-    <t>LightSlateGrey</t>
-  </si>
-  <si>
     <t>LightSteelBlue</t>
   </si>
   <si>
@@ -789,12 +747,6 @@
     <t>A0522D</t>
   </si>
   <si>
-    <t>Silver</t>
-  </si>
-  <si>
-    <t>C0C0C0</t>
-  </si>
-  <si>
     <t>SkyBlue</t>
   </si>
   <si>
@@ -807,15 +759,6 @@
     <t>6A5ACD</t>
   </si>
   <si>
-    <t>SlateGray</t>
-  </si>
-  <si>
-    <t>708090</t>
-  </si>
-  <si>
-    <t>SlateGrey</t>
-  </si>
-  <si>
     <t>Snow</t>
   </si>
   <si>
@@ -963,9 +906,6 @@
     <t>184,134,11</t>
   </si>
   <si>
-    <t>169,169,169</t>
-  </si>
-  <si>
     <t>0,100,0</t>
   </si>
   <si>
@@ -1011,9 +951,6 @@
     <t>0,191,255</t>
   </si>
   <si>
-    <t>105,105,105</t>
-  </si>
-  <si>
     <t>30,144,255</t>
   </si>
   <si>
@@ -1029,9 +966,6 @@
     <t>255,0,255</t>
   </si>
   <si>
-    <t>220,220,220</t>
-  </si>
-  <si>
     <t>248,248,255</t>
   </si>
   <si>
@@ -1041,9 +975,6 @@
     <t>218,165,32</t>
   </si>
   <si>
-    <t>128,128,128</t>
-  </si>
-  <si>
     <t>0,128,0</t>
   </si>
   <si>
@@ -1092,9 +1023,6 @@
     <t>250,250,210</t>
   </si>
   <si>
-    <t>211,211,211</t>
-  </si>
-  <si>
     <t>144,238,144</t>
   </si>
   <si>
@@ -1110,9 +1038,6 @@
     <t>135,206,250</t>
   </si>
   <si>
-    <t>119,136,153</t>
-  </si>
-  <si>
     <t>176,196,222</t>
   </si>
   <si>
@@ -1257,18 +1182,12 @@
     <t>160,82,45</t>
   </si>
   <si>
-    <t>192,192,192</t>
-  </si>
-  <si>
     <t>135,206,235</t>
   </si>
   <si>
     <t>106,90,205</t>
   </si>
   <si>
-    <t>112,128,144</t>
-  </si>
-  <si>
     <t>255,250,250</t>
   </si>
   <si>
@@ -1335,10 +1254,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Gray</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Classification</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1353,6 +1268,270 @@
   <si>
     <t>Orange</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5PB38</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20,72,125</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5B56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>44,131,153</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10BG44</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>45,104,110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10BG34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12,79,86</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5BG34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17,79,77</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10G34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>26,80,68</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5G34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>35,79,61</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5Y56</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>142,119,42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5Y46</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>115,94,20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10YR710</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>224,162,50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10YR610</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>195,136,15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10RP310</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>137,22,65</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10P94</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>248,218,238</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10P88</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10P714</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>244,134,220</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>243,180,226</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10B34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>37,75,98</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AP5</t>
+  </si>
+  <si>
+    <t>255,160,64</t>
+  </si>
+  <si>
+    <t>AP6</t>
+  </si>
+  <si>
+    <t>255,160,96</t>
+  </si>
+  <si>
+    <t>AP7</t>
+  </si>
+  <si>
+    <t>255,160,160</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AP8</t>
+  </si>
+  <si>
+    <t>255,192,160</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AP9</t>
+  </si>
+  <si>
+    <t>255,96,0</t>
+  </si>
+  <si>
+    <t>AP10</t>
+  </si>
+  <si>
+    <t>255,96,128</t>
+  </si>
+  <si>
+    <t>AP11</t>
+  </si>
+  <si>
+    <t>224,255,64</t>
+  </si>
+  <si>
+    <t>AP12</t>
+  </si>
+  <si>
+    <t>224,160,160</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AP13</t>
+  </si>
+  <si>
+    <t>AP14</t>
+  </si>
+  <si>
+    <t>224,64,32</t>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AP15</t>
+  </si>
+  <si>
+    <t>224,0,192</t>
+  </si>
+  <si>
+    <t>AP16</t>
+  </si>
+  <si>
+    <t>192,192,32</t>
+  </si>
+  <si>
+    <t>AP17</t>
+  </si>
+  <si>
+    <t>192,255,192</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AP18</t>
+  </si>
+  <si>
+    <t>192,192,0</t>
+  </si>
+  <si>
+    <t>AP19</t>
+  </si>
+  <si>
+    <t>160,192,96</t>
+  </si>
+  <si>
+    <t>AP20</t>
+  </si>
+  <si>
+    <t>160,224,192</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AP21</t>
+  </si>
+  <si>
+    <t>128,64,96</t>
+  </si>
+  <si>
+    <t>AP22</t>
+  </si>
+  <si>
+    <t>128,96,160</t>
+  </si>
+  <si>
+    <t>AP23</t>
+  </si>
+  <si>
+    <t>96,64,64</t>
+  </si>
+  <si>
+    <t>AP24</t>
+  </si>
+  <si>
+    <t>64,64,160</t>
+  </si>
+  <si>
+    <t>AP25</t>
+  </si>
+  <si>
+    <t>64,0,0</t>
   </si>
 </sst>
 </file>
@@ -1442,8 +1621,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E9C9674-90CE-4D8F-B127-5F27C9B931F5}" name="表_1" displayName="表_1" ref="A1:D145" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D145" xr:uid="{5E9C9674-90CE-4D8F-B127-5F27C9B931F5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E9C9674-90CE-4D8F-B127-5F27C9B931F5}" name="表_1" displayName="表_1" ref="A1:D171" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D171" xr:uid="{5E9C9674-90CE-4D8F-B127-5F27C9B931F5}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A71A95BF-58BF-4D55-8E8C-2208518EE4D6}" uniqueName="1" name="Colorname" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{E612895B-8433-425C-99DA-B7549524A36F}" uniqueName="2" name="HEX" queryTableFieldId="2" dataDxfId="2"/>
@@ -1719,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41BA6CDF-51E5-4163-9A88-E70DDB856298}">
   <dimension ref="A1:D171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="G123" sqref="G123"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1733,7 +1912,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>424</v>
+        <v>397</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1742,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>431</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1753,10 +1932,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="D2" t="s">
-        <v>429</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1767,7 +1946,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>286</v>
+        <v>267</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -1781,10 +1960,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="D4" t="s">
-        <v>432</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1795,10 +1974,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>288</v>
+        <v>269</v>
       </c>
       <c r="D5" t="s">
-        <v>433</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1809,10 +1988,10 @@
         <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="D6" t="s">
-        <v>429</v>
+        <v>402</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1823,10 +2002,10 @@
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>290</v>
+        <v>271</v>
       </c>
       <c r="D7" t="s">
-        <v>429</v>
+        <v>402</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1837,10 +2016,10 @@
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="D8" t="s">
-        <v>426</v>
+        <v>399</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1851,7 +2030,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
@@ -1865,10 +2044,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>293</v>
+        <v>274</v>
       </c>
       <c r="D10" t="s">
-        <v>426</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1879,7 +2058,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -1893,7 +2072,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="D12" t="s">
         <v>26</v>
@@ -1907,7 +2086,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
@@ -1921,10 +2100,10 @@
         <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="D14" t="s">
-        <v>426</v>
+        <v>399</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1935,10 +2114,10 @@
         <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="D15" t="s">
-        <v>432</v>
+        <v>404</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1949,7 +2128,7 @@
         <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="D16" t="s">
         <v>35</v>
@@ -1963,10 +2142,10 @@
         <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
       <c r="D17" t="s">
-        <v>434</v>
+        <v>406</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1977,7 +2156,7 @@
         <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
       <c r="D18" t="s">
         <v>40</v>
@@ -1991,7 +2170,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>302</v>
+        <v>283</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -2005,10 +2184,10 @@
         <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="D20" t="s">
-        <v>426</v>
+        <v>399</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2019,7 +2198,7 @@
         <v>46</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>304</v>
+        <v>285</v>
       </c>
       <c r="D21" t="s">
         <v>47</v>
@@ -2033,10 +2212,10 @@
         <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="D22" t="s">
-        <v>432</v>
+        <v>404</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2047,7 +2226,7 @@
         <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>305</v>
+        <v>286</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -2061,10 +2240,10 @@
         <v>51</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="D24" t="s">
-        <v>433</v>
+        <v>405</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2075,10 +2254,10 @@
         <v>53</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="D25" t="s">
-        <v>426</v>
+        <v>399</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2089,178 +2268,178 @@
         <v>56</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
         <v>58</v>
       </c>
-      <c r="B27" t="s">
-        <v>59</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="D27" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
         <v>60</v>
       </c>
-      <c r="B28" t="s">
-        <v>61</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>310</v>
+        <v>291</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
         <v>62</v>
       </c>
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>311</v>
+        <v>292</v>
       </c>
       <c r="D29" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
         <v>64</v>
       </c>
-      <c r="B30" t="s">
-        <v>65</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
         <v>66</v>
       </c>
-      <c r="B31" t="s">
-        <v>67</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>313</v>
+        <v>294</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" t="s">
         <v>68</v>
       </c>
-      <c r="B32" t="s">
-        <v>69</v>
-      </c>
       <c r="C32" s="1" t="s">
-        <v>314</v>
+        <v>295</v>
       </c>
       <c r="D32" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" t="s">
         <v>70</v>
       </c>
-      <c r="B33" t="s">
-        <v>71</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>315</v>
+        <v>296</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
         <v>72</v>
       </c>
-      <c r="B34" t="s">
-        <v>73</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>316</v>
+        <v>297</v>
       </c>
       <c r="D34" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" t="s">
         <v>74</v>
       </c>
-      <c r="B35" t="s">
-        <v>75</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>401</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" t="s">
         <v>76</v>
       </c>
-      <c r="B36" t="s">
-        <v>77</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>318</v>
+        <v>299</v>
       </c>
       <c r="D36" t="s">
-        <v>428</v>
+        <v>405</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" t="s">
         <v>78</v>
       </c>
-      <c r="B37" t="s">
-        <v>79</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="D37" t="s">
-        <v>432</v>
+        <v>404</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" t="s">
         <v>80</v>
       </c>
-      <c r="B38" t="s">
-        <v>79</v>
-      </c>
       <c r="C38" s="1" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="D38" t="s">
-        <v>432</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2271,38 +2450,38 @@
         <v>82</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="D39" t="s">
-        <v>432</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="D40" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="D41" t="s">
-        <v>87</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2313,10 +2492,10 @@
         <v>89</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="D42" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2327,10 +2506,10 @@
         <v>91</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="D43" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2341,10 +2520,10 @@
         <v>93</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="D44" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2355,10 +2534,10 @@
         <v>95</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="D45" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2369,7 +2548,7 @@
         <v>97</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
@@ -2383,10 +2562,10 @@
         <v>99</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="D47" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2397,388 +2576,388 @@
         <v>101</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="D48" t="s">
-        <v>26</v>
+        <v>400</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" t="s">
         <v>102</v>
       </c>
-      <c r="B49" t="s">
-        <v>103</v>
-      </c>
       <c r="C49" s="1" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
       <c r="D49" t="s">
-        <v>430</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" t="s">
         <v>104</v>
       </c>
-      <c r="B50" t="s">
-        <v>105</v>
-      </c>
       <c r="C50" s="1" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" t="s">
         <v>106</v>
       </c>
-      <c r="B51" t="s">
-        <v>107</v>
-      </c>
       <c r="C51" s="1" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
       <c r="D51" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>107</v>
+      </c>
+      <c r="B52" t="s">
         <v>108</v>
       </c>
-      <c r="B52" t="s">
-        <v>109</v>
-      </c>
       <c r="C52" s="1" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="D52" t="s">
-        <v>434</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B53" t="s">
         <v>110</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>334</v>
+        <v>316</v>
       </c>
       <c r="D53" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="D54" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="D55" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>400</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B57" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
       <c r="D57" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="D58" t="s">
-        <v>47</v>
+        <v>402</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
       <c r="D59" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="D60" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B61" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="D61" t="s">
-        <v>427</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B62" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
       <c r="D62" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>344</v>
+        <v>326</v>
       </c>
       <c r="D63" t="s">
-        <v>429</v>
+        <v>404</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B64" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>345</v>
+        <v>327</v>
       </c>
       <c r="D64" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B65" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
       <c r="D65" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B66" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="D66" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B67" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>348</v>
+        <v>330</v>
       </c>
       <c r="D67" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B68" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>349</v>
+        <v>331</v>
       </c>
       <c r="D68" t="s">
-        <v>432</v>
+        <v>405</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B69" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="D69" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B70" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>351</v>
+        <v>333</v>
       </c>
       <c r="D70" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B71" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
       <c r="D71" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B72" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>353</v>
+        <v>335</v>
       </c>
       <c r="D72" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B73" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>354</v>
+        <v>336</v>
       </c>
       <c r="D73" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B74" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>355</v>
+        <v>337</v>
       </c>
       <c r="D74" t="s">
-        <v>433</v>
+        <v>402</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B75" t="s">
-        <v>153</v>
+        <v>95</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>356</v>
+        <v>308</v>
       </c>
       <c r="D75" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2789,10 +2968,10 @@
         <v>155</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="D76" t="s">
-        <v>57</v>
+        <v>399</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2800,24 +2979,24 @@
         <v>156</v>
       </c>
       <c r="B77" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>357</v>
+        <v>339</v>
       </c>
       <c r="D77" t="s">
-        <v>57</v>
+        <v>405</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B78" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>358</v>
+        <v>340</v>
       </c>
       <c r="D78" t="s">
         <v>4</v>
@@ -2825,41 +3004,41 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B79" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="D79" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B80" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="D80" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B81" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="D81" t="s">
         <v>35</v>
@@ -2867,69 +3046,69 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B82" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>362</v>
+        <v>344</v>
       </c>
       <c r="D82" t="s">
-        <v>429</v>
+        <v>401</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B83" t="s">
-        <v>101</v>
+        <v>169</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>329</v>
+        <v>345</v>
       </c>
       <c r="D83" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B84" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>363</v>
+        <v>346</v>
       </c>
       <c r="D84" t="s">
-        <v>426</v>
+        <v>404</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B85" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>364</v>
+        <v>347</v>
       </c>
       <c r="D85" t="s">
-        <v>433</v>
+        <v>398</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B86" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>365</v>
+        <v>348</v>
       </c>
       <c r="D86" t="s">
         <v>4</v>
@@ -2937,310 +3116,310 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B87" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>366</v>
+        <v>349</v>
       </c>
       <c r="D87" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B88" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>367</v>
+        <v>350</v>
       </c>
       <c r="D88" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B89" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>368</v>
+        <v>351</v>
       </c>
       <c r="D89" t="s">
-        <v>35</v>
+        <v>400</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B90" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>369</v>
+        <v>352</v>
       </c>
       <c r="D90" t="s">
-        <v>428</v>
+        <v>399</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B91" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>370</v>
+        <v>353</v>
       </c>
       <c r="D91" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B92" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>371</v>
+        <v>354</v>
       </c>
       <c r="D92" t="s">
-        <v>432</v>
+        <v>402</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B93" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>372</v>
+        <v>355</v>
       </c>
       <c r="D93" t="s">
-        <v>425</v>
+        <v>35</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B94" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>373</v>
+        <v>356</v>
       </c>
       <c r="D94" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>190</v>
+        <v>40</v>
       </c>
       <c r="B95" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>374</v>
+        <v>357</v>
       </c>
       <c r="D95" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B96" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>375</v>
+        <v>358</v>
       </c>
       <c r="D96" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B97" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>376</v>
+        <v>359</v>
       </c>
       <c r="D97" t="s">
-        <v>427</v>
+        <v>26</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B98" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>377</v>
+        <v>360</v>
       </c>
       <c r="D98" t="s">
-        <v>426</v>
+        <v>54</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B99" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>378</v>
+        <v>361</v>
       </c>
       <c r="D99" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B100" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>379</v>
+        <v>362</v>
       </c>
       <c r="D100" t="s">
-        <v>429</v>
+        <v>404</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B101" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>380</v>
+        <v>363</v>
       </c>
       <c r="D101" t="s">
-        <v>35</v>
+        <v>398</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B102" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>381</v>
+        <v>364</v>
       </c>
       <c r="D102" t="s">
-        <v>35</v>
+        <v>400</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>40</v>
+        <v>207</v>
       </c>
       <c r="B103" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>382</v>
+        <v>365</v>
       </c>
       <c r="D103" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B104" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
       <c r="D104" t="s">
-        <v>47</v>
+        <v>399</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>209</v>
+        <v>83</v>
       </c>
       <c r="B105" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>384</v>
+        <v>367</v>
       </c>
       <c r="D105" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B106" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>385</v>
+        <v>368</v>
       </c>
       <c r="D106" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B107" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>386</v>
+        <v>369</v>
       </c>
       <c r="D107" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>215</v>
+        <v>26</v>
       </c>
       <c r="B108" t="s">
         <v>216</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>387</v>
+        <v>370</v>
       </c>
       <c r="D108" t="s">
-        <v>432</v>
+        <v>26</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3251,66 +3430,66 @@
         <v>218</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>388</v>
+        <v>371</v>
       </c>
       <c r="D109" t="s">
-        <v>425</v>
+        <v>26</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>47</v>
+      </c>
+      <c r="B110" t="s">
         <v>219</v>
       </c>
-      <c r="B110" t="s">
-        <v>220</v>
-      </c>
       <c r="C110" s="1" t="s">
-        <v>389</v>
+        <v>372</v>
       </c>
       <c r="D110" t="s">
-        <v>427</v>
+        <v>47</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" t="s">
         <v>221</v>
       </c>
-      <c r="B111" t="s">
-        <v>222</v>
-      </c>
       <c r="C111" s="1" t="s">
-        <v>390</v>
+        <v>373</v>
       </c>
       <c r="D111" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>222</v>
+      </c>
+      <c r="B112" t="s">
         <v>223</v>
       </c>
-      <c r="B112" t="s">
-        <v>224</v>
-      </c>
       <c r="C112" s="1" t="s">
-        <v>391</v>
+        <v>374</v>
       </c>
       <c r="D112" t="s">
-        <v>426</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>87</v>
+        <v>224</v>
       </c>
       <c r="B113" t="s">
         <v>225</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
       <c r="D113" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -3321,10 +3500,10 @@
         <v>227</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
       <c r="D114" t="s">
-        <v>26</v>
+        <v>398</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3335,245 +3514,245 @@
         <v>229</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
       <c r="D115" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>26</v>
+        <v>230</v>
       </c>
       <c r="B116" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
       <c r="D116" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B117" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="D117" t="s">
-        <v>26</v>
+        <v>402</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>47</v>
+        <v>234</v>
       </c>
       <c r="B118" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>397</v>
+        <v>380</v>
       </c>
       <c r="D118" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B119" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
       <c r="D119" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B120" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>399</v>
+        <v>382</v>
       </c>
       <c r="D120" t="s">
-        <v>4</v>
+        <v>401</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B121" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>400</v>
+        <v>383</v>
       </c>
       <c r="D121" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B122" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>401</v>
+        <v>384</v>
       </c>
       <c r="D122" t="s">
-        <v>425</v>
+        <v>35</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B123" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>402</v>
+        <v>385</v>
       </c>
       <c r="D123" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B124" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>403</v>
+        <v>386</v>
       </c>
       <c r="D124" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B125" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>404</v>
+        <v>387</v>
       </c>
       <c r="D125" t="s">
-        <v>429</v>
+        <v>405</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B126" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
       <c r="D126" t="s">
-        <v>27</v>
+        <v>401</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B127" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="D127" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B128" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="D128" t="s">
-        <v>4</v>
+        <v>404</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B129" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
       <c r="D129" t="s">
-        <v>428</v>
+        <v>26</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B130" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>409</v>
+        <v>392</v>
       </c>
       <c r="D130" t="s">
-        <v>57</v>
+        <v>399</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>258</v>
+        <v>7</v>
       </c>
       <c r="B131" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="D131" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B132" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="D132" t="s">
         <v>7</v>
@@ -3581,263 +3760,501 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>261</v>
+        <v>54</v>
       </c>
       <c r="B133" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="D133" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B134" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="D134" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>265</v>
-      </c>
-      <c r="B135" t="s">
-        <v>266</v>
+        <v>407</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D135" t="s">
-        <v>27</v>
+        <v>404</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>267</v>
-      </c>
-      <c r="B136" t="s">
-        <v>268</v>
+        <v>409</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D136" t="s">
-        <v>433</v>
+        <v>404</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>269</v>
-      </c>
-      <c r="B137" t="s">
-        <v>270</v>
+        <v>437</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>415</v>
+        <v>438</v>
       </c>
       <c r="D137" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>271</v>
-      </c>
-      <c r="B138" t="s">
-        <v>272</v>
+        <v>411</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D138" t="s">
-        <v>47</v>
+        <v>405</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>273</v>
-      </c>
-      <c r="B139" t="s">
-        <v>274</v>
+        <v>413</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D139" t="s">
-        <v>432</v>
+        <v>405</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>275</v>
-      </c>
-      <c r="B140" t="s">
-        <v>276</v>
+        <v>415</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D140" t="s">
-        <v>26</v>
+        <v>405</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>277</v>
-      </c>
-      <c r="B141" t="s">
-        <v>278</v>
+        <v>417</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D141" t="s">
-        <v>426</v>
+        <v>405</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>7</v>
-      </c>
-      <c r="B142" t="s">
-        <v>279</v>
+        <v>419</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>420</v>
       </c>
       <c r="D142" t="s">
-        <v>7</v>
+        <v>405</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>280</v>
-      </c>
-      <c r="B143" t="s">
-        <v>281</v>
+        <v>421</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D143" t="s">
-        <v>7</v>
+        <v>399</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>54</v>
-      </c>
-      <c r="B144" t="s">
-        <v>282</v>
+        <v>423</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D144" t="s">
-        <v>54</v>
+        <v>399</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>283</v>
-      </c>
-      <c r="B145" t="s">
-        <v>284</v>
+        <v>425</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="D145" t="s">
-        <v>35</v>
+        <v>406</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C146" s="1"/>
+      <c r="A146" t="s">
+        <v>427</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D146" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C147" s="1"/>
+      <c r="A147" t="s">
+        <v>429</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D147" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C148" s="1"/>
+      <c r="A148" t="s">
+        <v>431</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D148" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C149" s="1"/>
+      <c r="A149" t="s">
+        <v>433</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D149" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C150" s="1"/>
+      <c r="A150" t="s">
+        <v>434</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D150" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C151" s="1"/>
+      <c r="A151" t="s">
+        <v>440</v>
+      </c>
+      <c r="B151" t="s">
+        <v>439</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D151" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C152" s="1"/>
+      <c r="A152" t="s">
+        <v>442</v>
+      </c>
+      <c r="B152" t="s">
+        <v>439</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D152" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C153" s="1"/>
+      <c r="A153" t="s">
+        <v>444</v>
+      </c>
+      <c r="B153" t="s">
+        <v>439</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="D153" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C154" s="1"/>
+      <c r="A154" t="s">
+        <v>446</v>
+      </c>
+      <c r="B154" t="s">
+        <v>439</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D154" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C155" s="1"/>
+      <c r="A155" t="s">
+        <v>448</v>
+      </c>
+      <c r="B155" t="s">
+        <v>439</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="D155" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C156" s="1"/>
+      <c r="A156" t="s">
+        <v>450</v>
+      </c>
+      <c r="B156" t="s">
+        <v>439</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="D156" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C157" s="1"/>
+      <c r="A157" t="s">
+        <v>452</v>
+      </c>
+      <c r="B157" t="s">
+        <v>439</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="D157" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C158" s="1"/>
+      <c r="A158" t="s">
+        <v>454</v>
+      </c>
+      <c r="B158" t="s">
+        <v>439</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D158" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C159" s="1"/>
+      <c r="A159" t="s">
+        <v>456</v>
+      </c>
+      <c r="B159" t="s">
+        <v>439</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D159" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C160" s="1"/>
-    </row>
-    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C161" s="1"/>
-    </row>
-    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C162" s="1"/>
-    </row>
-    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C163" s="1"/>
-    </row>
-    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C164" s="1"/>
-    </row>
-    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C165" s="1"/>
-    </row>
-    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C166" s="1"/>
-    </row>
-    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C167" s="1"/>
-    </row>
-    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C168" s="1"/>
-    </row>
-    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C169" s="1"/>
-    </row>
-    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C170" s="1"/>
-    </row>
-    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C171" s="1"/>
+      <c r="A160" t="s">
+        <v>457</v>
+      </c>
+      <c r="B160" t="s">
+        <v>439</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D160" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>460</v>
+      </c>
+      <c r="B161" t="s">
+        <v>439</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D161" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>462</v>
+      </c>
+      <c r="B162" t="s">
+        <v>439</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D162" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>464</v>
+      </c>
+      <c r="B163" t="s">
+        <v>439</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D163" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>466</v>
+      </c>
+      <c r="B164" t="s">
+        <v>439</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="D164" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>468</v>
+      </c>
+      <c r="B165" t="s">
+        <v>439</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="D165" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>470</v>
+      </c>
+      <c r="B166" t="s">
+        <v>439</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D166" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>472</v>
+      </c>
+      <c r="B167" t="s">
+        <v>439</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="D167" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>474</v>
+      </c>
+      <c r="B168" t="s">
+        <v>439</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="D168" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>476</v>
+      </c>
+      <c r="B169" t="s">
+        <v>439</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D169" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>478</v>
+      </c>
+      <c r="B170" t="s">
+        <v>439</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D170" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>480</v>
+      </c>
+      <c r="B171" t="s">
+        <v>439</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="D171" t="s">
+        <v>399</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>